<commit_message>
More naming rationalisation. More sensible sequence size handling since buildSequence() was moved.
</commit_message>
<xml_diff>
--- a/Documents/System diagrams.xlsx
+++ b/Documents/System diagrams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975" tabRatio="617" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9975" tabRatio="617" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Existing Init" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="64">
   <si>
     <t>x</t>
   </si>
@@ -1432,7 +1432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1725,8 +1725,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1768,6 +1768,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1809,6 +1812,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1974,18 +1995,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2148,12 +2157,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2178,12 +2181,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2209,6 +2206,42 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6164,15 +6197,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>226358</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>151283</xdr:rowOff>
+      <xdr:colOff>215152</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>207312</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>504264</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:colOff>493058</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6181,7 +6214,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4574240" y="6415371"/>
+          <a:off x="4563034" y="6236077"/>
           <a:ext cx="1510553" cy="857247"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6658,16 +6691,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>107575</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>5042</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>802339</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>83482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>145677</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1355912</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6676,8 +6709,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4612340" y="6863042"/>
-          <a:ext cx="2055160" cy="1149164"/>
+          <a:off x="2931457" y="2134158"/>
+          <a:ext cx="1528484" cy="1631019"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7378,15 +7411,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>528359</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>70036</xdr:rowOff>
+      <xdr:colOff>606800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>134469</xdr:rowOff>
+      <xdr:colOff>1030941</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7395,8 +7428,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7677712" y="3880036"/>
-          <a:ext cx="2497229" cy="445433"/>
+          <a:off x="7554447" y="3095624"/>
+          <a:ext cx="2497229" cy="613523"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7427,7 +7460,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> by eCAN hardware and not stored in any mailbox.</a:t>
+            <a:t> by eCAN hardware and not stored in any mailbox. No software processing is necessary.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -7827,10 +7860,10 @@
       <c r="B5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="46"/>
-      <c r="H5" s="157" t="s">
+      <c r="H5" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="157"/>
+      <c r="I5" s="164"/>
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -7878,10 +7911,10 @@
       <c r="F10" s="32"/>
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
-      <c r="I10" s="158" t="s">
+      <c r="I10" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="159"/>
+      <c r="J10" s="166"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
@@ -7897,10 +7930,10 @@
       <c r="E12" s="25"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="164" t="s">
+      <c r="H12" s="171" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="165"/>
+      <c r="I12" s="172"/>
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -7908,8 +7941,8 @@
       <c r="E13" s="25"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="166"/>
-      <c r="I13" s="167"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="174"/>
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -7932,17 +7965,17 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
-      <c r="C16" s="160" t="s">
+      <c r="C16" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
       <c r="F16" s="22"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="161" t="s">
+      <c r="H16" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="161"/>
+      <c r="I16" s="168"/>
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -8207,16 +8240,16 @@
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="162" t="s">
+      <c r="E37" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="163"/>
+      <c r="F37" s="170"/>
       <c r="G37" s="26"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="162" t="s">
+      <c r="I37" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="163"/>
+      <c r="J37" s="170"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -8241,7 +8274,7 @@
   <dimension ref="B2:J38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8296,10 +8329,10 @@
       <c r="B5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="46"/>
-      <c r="H5" s="157" t="s">
+      <c r="H5" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="157"/>
+      <c r="I5" s="164"/>
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -8351,10 +8384,10 @@
       <c r="F10" s="32"/>
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
-      <c r="I10" s="158" t="s">
+      <c r="I10" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="159"/>
+      <c r="J10" s="166"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
@@ -8370,10 +8403,10 @@
       <c r="E12" s="25"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="168" t="s">
+      <c r="H12" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="169"/>
+      <c r="I12" s="176"/>
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -8381,8 +8414,8 @@
       <c r="E13" s="25"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="170"/>
-      <c r="I13" s="171"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="178"/>
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -8405,17 +8438,17 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
-      <c r="C16" s="160" t="s">
+      <c r="C16" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
       <c r="F16" s="22"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="161" t="s">
+      <c r="H16" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="161"/>
+      <c r="I16" s="168"/>
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -8682,16 +8715,16 @@
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="162" t="s">
+      <c r="E37" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="163"/>
+      <c r="F37" s="170"/>
       <c r="G37" s="26"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="162" t="s">
+      <c r="I37" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="163"/>
+      <c r="J37" s="170"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -8771,10 +8804,10 @@
       <c r="B5" s="19"/>
       <c r="F5" s="20"/>
       <c r="G5" s="46"/>
-      <c r="H5" s="157" t="s">
+      <c r="H5" s="164" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="157"/>
+      <c r="I5" s="164"/>
       <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -8826,10 +8859,10 @@
       <c r="F10" s="32"/>
       <c r="G10" s="56"/>
       <c r="H10" s="57"/>
-      <c r="I10" s="158" t="s">
+      <c r="I10" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="159"/>
+      <c r="J10" s="166"/>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
@@ -8845,10 +8878,10 @@
       <c r="E12" s="25"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="168" t="s">
+      <c r="H12" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="169"/>
+      <c r="I12" s="176"/>
       <c r="J12" s="22"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -8856,8 +8889,8 @@
       <c r="E13" s="25"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="170"/>
-      <c r="I13" s="171"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="178"/>
       <c r="J13" s="22"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -8880,17 +8913,17 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
-      <c r="C16" s="160" t="s">
+      <c r="C16" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="160"/>
-      <c r="E16" s="160"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="167"/>
       <c r="F16" s="22"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="161" t="s">
+      <c r="H16" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="161"/>
+      <c r="I16" s="168"/>
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -9155,16 +9188,16 @@
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="162" t="s">
+      <c r="E37" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="163"/>
+      <c r="F37" s="170"/>
       <c r="G37" s="26"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="162" t="s">
+      <c r="I37" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="163"/>
+      <c r="J37" s="170"/>
     </row>
     <row r="38" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -9251,20 +9284,20 @@
     </row>
     <row r="5" spans="2:28" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
-      <c r="C5" s="160" t="s">
+      <c r="C5" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
       <c r="F5" s="99"/>
       <c r="G5" s="99"/>
       <c r="H5" s="20"/>
       <c r="I5" s="46"/>
-      <c r="J5" s="174" t="s">
+      <c r="J5" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
       <c r="M5" s="109"/>
       <c r="N5" s="47"/>
       <c r="T5" s="111"/>
@@ -9279,30 +9312,30 @@
     </row>
     <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="118" t="s">
+      <c r="D6" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="118" t="s">
+      <c r="E6" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="118" t="s">
+      <c r="F6" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="118" t="s">
+      <c r="G6" s="119" t="s">
         <v>57</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="48"/>
-      <c r="J6" s="148" t="s">
+      <c r="J6" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="148" t="s">
+      <c r="K6" s="155" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="148" t="s">
+      <c r="L6" s="155" t="s">
         <v>4</v>
       </c>
       <c r="M6" s="70"/>
@@ -9319,29 +9352,29 @@
     </row>
     <row r="7" spans="2:28" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
-      <c r="C7" s="136">
+      <c r="C7" s="143">
         <v>0</v>
       </c>
-      <c r="D7" s="137" t="s">
+      <c r="D7" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="138"/>
-      <c r="F7" s="139">
+      <c r="E7" s="145"/>
+      <c r="F7" s="146">
         <v>0</v>
       </c>
-      <c r="G7" s="140">
+      <c r="G7" s="147">
         <v>1</v>
       </c>
-      <c r="H7" s="134"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="149">
+      <c r="H7" s="141"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="156">
         <v>0</v>
       </c>
-      <c r="K7" s="150" t="s">
+      <c r="K7" s="157" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="151"/>
-      <c r="M7" s="185"/>
+      <c r="L7" s="158"/>
+      <c r="M7" s="188"/>
       <c r="N7" s="50"/>
       <c r="T7" s="25"/>
       <c r="U7" s="25"/>
@@ -9355,7 +9388,7 @@
     </row>
     <row r="8" spans="2:28" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
-      <c r="C8" s="132">
+      <c r="C8" s="139">
         <v>1</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -9365,19 +9398,19 @@
       <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8" s="133">
+      <c r="G8" s="140">
         <v>1</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="59"/>
-      <c r="J8" s="152">
+      <c r="J8" s="159">
         <v>1</v>
       </c>
       <c r="K8" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="153"/>
-      <c r="M8" s="116"/>
+      <c r="L8" s="160"/>
+      <c r="M8" s="117"/>
       <c r="N8" s="50"/>
       <c r="T8" s="25"/>
       <c r="U8" s="25"/>
@@ -9391,17 +9424,17 @@
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
-      <c r="C9" s="132"/>
+      <c r="C9" s="139"/>
       <c r="D9" s="12"/>
       <c r="E9" s="6"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="133"/>
+      <c r="G9" s="140"/>
       <c r="H9" s="23"/>
       <c r="I9" s="59"/>
-      <c r="J9" s="152"/>
+      <c r="J9" s="159"/>
       <c r="K9" s="58"/>
-      <c r="L9" s="153"/>
-      <c r="M9" s="185"/>
+      <c r="L9" s="160"/>
+      <c r="M9" s="188"/>
       <c r="N9" s="50"/>
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
@@ -9415,17 +9448,17 @@
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
-      <c r="C10" s="132"/>
+      <c r="C10" s="139"/>
       <c r="D10" s="12"/>
       <c r="E10" s="6"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="133"/>
+      <c r="G10" s="140"/>
       <c r="H10" s="23"/>
       <c r="I10" s="59"/>
-      <c r="J10" s="152"/>
+      <c r="J10" s="159"/>
       <c r="K10" s="58"/>
-      <c r="L10" s="153"/>
-      <c r="M10" s="185"/>
+      <c r="L10" s="160"/>
+      <c r="M10" s="188"/>
       <c r="N10" s="50"/>
       <c r="T10" s="25"/>
       <c r="U10" s="25"/>
@@ -9439,17 +9472,17 @@
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
-      <c r="C11" s="132"/>
+      <c r="C11" s="139"/>
       <c r="D11" s="12"/>
       <c r="E11" s="6"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="133"/>
+      <c r="G11" s="140"/>
       <c r="H11" s="23"/>
       <c r="I11" s="59"/>
-      <c r="J11" s="152"/>
+      <c r="J11" s="159"/>
       <c r="K11" s="58"/>
-      <c r="L11" s="153"/>
-      <c r="M11" s="185"/>
+      <c r="L11" s="160"/>
+      <c r="M11" s="188"/>
       <c r="N11" s="50"/>
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
@@ -9463,17 +9496,17 @@
     </row>
     <row r="12" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21"/>
-      <c r="C12" s="141"/>
+      <c r="C12" s="148"/>
       <c r="D12" s="12"/>
       <c r="E12" s="6"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="133"/>
+      <c r="G12" s="140"/>
       <c r="H12" s="23"/>
       <c r="I12" s="59"/>
-      <c r="J12" s="152"/>
+      <c r="J12" s="159"/>
       <c r="K12" s="58"/>
-      <c r="L12" s="153"/>
-      <c r="M12" s="185"/>
+      <c r="L12" s="160"/>
+      <c r="M12" s="188"/>
       <c r="N12" s="50"/>
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
@@ -9487,29 +9520,29 @@
     </row>
     <row r="13" spans="2:28" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="21"/>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="142" t="s">
+      <c r="D13" s="149" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="143"/>
-      <c r="F13" s="144">
+      <c r="E13" s="150"/>
+      <c r="F13" s="151">
         <v>0</v>
       </c>
-      <c r="G13" s="145">
+      <c r="G13" s="152">
         <v>1</v>
       </c>
-      <c r="H13" s="135"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="154" t="s">
+      <c r="H13" s="142"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="155" t="s">
+      <c r="K13" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="156"/>
-      <c r="M13" s="185"/>
+      <c r="L13" s="163"/>
+      <c r="M13" s="188"/>
       <c r="N13" s="50"/>
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
@@ -9529,11 +9562,11 @@
       <c r="D14" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="198"/>
-      <c r="F14" s="136">
+      <c r="E14" s="201"/>
+      <c r="F14" s="143">
         <v>1</v>
       </c>
-      <c r="G14" s="140">
+      <c r="G14" s="147">
         <v>1</v>
       </c>
       <c r="H14" s="22"/>
@@ -9557,9 +9590,9 @@
       <c r="B15" s="21"/>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="199"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="133"/>
+      <c r="E15" s="202"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="140"/>
       <c r="H15" s="22"/>
       <c r="I15" s="54"/>
       <c r="J15" s="55"/>
@@ -9581,9 +9614,9 @@
       <c r="B16" s="21"/>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="199"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="133"/>
+      <c r="E16" s="202"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="140"/>
       <c r="H16" s="22"/>
       <c r="I16" s="54"/>
       <c r="J16" s="54"/>
@@ -9605,9 +9638,9 @@
       <c r="B17" s="21"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="199"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="133"/>
+      <c r="E17" s="202"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="140"/>
       <c r="H17" s="22"/>
       <c r="I17" s="54"/>
       <c r="J17" s="54"/>
@@ -9629,9 +9662,9 @@
       <c r="B18" s="21"/>
       <c r="C18" s="2"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="199"/>
-      <c r="F18" s="132"/>
-      <c r="G18" s="133"/>
+      <c r="E18" s="202"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="140"/>
       <c r="H18" s="22"/>
       <c r="I18" s="54"/>
       <c r="J18" s="54"/>
@@ -9653,9 +9686,9 @@
       <c r="B19" s="21"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="199"/>
-      <c r="F19" s="132"/>
-      <c r="G19" s="133"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="140"/>
       <c r="H19" s="22"/>
       <c r="I19" s="54"/>
       <c r="J19" s="54"/>
@@ -9677,9 +9710,9 @@
       <c r="B20" s="21"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="199"/>
-      <c r="F20" s="132"/>
-      <c r="G20" s="133"/>
+      <c r="E20" s="202"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="140"/>
       <c r="H20" s="22"/>
       <c r="I20" s="54"/>
       <c r="J20" s="54"/>
@@ -9701,20 +9734,20 @@
       <c r="B21" s="21"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="199"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="133"/>
+      <c r="E21" s="202"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="140"/>
       <c r="H21" s="22"/>
       <c r="I21" s="54"/>
-      <c r="J21" s="172"/>
-      <c r="K21" s="172"/>
+      <c r="J21" s="179"/>
+      <c r="K21" s="179"/>
       <c r="L21" s="70"/>
       <c r="M21" s="70"/>
       <c r="N21" s="50"/>
       <c r="T21" s="25"/>
       <c r="U21" s="54"/>
-      <c r="V21" s="172"/>
-      <c r="W21" s="172"/>
+      <c r="V21" s="179"/>
+      <c r="W21" s="179"/>
       <c r="X21" s="70"/>
       <c r="Y21" s="54"/>
       <c r="Z21" s="25"/>
@@ -9725,20 +9758,20 @@
       <c r="B22" s="21"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="199"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="133"/>
+      <c r="E22" s="202"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="140"/>
       <c r="H22" s="22"/>
       <c r="I22" s="54"/>
-      <c r="J22" s="173"/>
-      <c r="K22" s="173"/>
+      <c r="J22" s="180"/>
+      <c r="K22" s="180"/>
       <c r="L22" s="68"/>
       <c r="M22" s="68"/>
       <c r="N22" s="50"/>
       <c r="T22" s="25"/>
       <c r="U22" s="54"/>
-      <c r="V22" s="173"/>
-      <c r="W22" s="173"/>
+      <c r="V22" s="180"/>
+      <c r="W22" s="180"/>
       <c r="X22" s="68"/>
       <c r="Y22" s="54"/>
       <c r="Z22" s="25"/>
@@ -9749,20 +9782,20 @@
       <c r="B23" s="21"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="199"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="133"/>
+      <c r="E23" s="202"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="140"/>
       <c r="H23" s="22"/>
       <c r="I23" s="54"/>
-      <c r="J23" s="173"/>
-      <c r="K23" s="173"/>
+      <c r="J23" s="180"/>
+      <c r="K23" s="180"/>
       <c r="L23" s="68"/>
       <c r="M23" s="68"/>
       <c r="N23" s="50"/>
       <c r="T23" s="25"/>
       <c r="U23" s="54"/>
-      <c r="V23" s="173"/>
-      <c r="W23" s="173"/>
+      <c r="V23" s="180"/>
+      <c r="W23" s="180"/>
       <c r="X23" s="68"/>
       <c r="Y23" s="54"/>
       <c r="Z23" s="25"/>
@@ -9777,11 +9810,11 @@
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="199"/>
-      <c r="F24" s="200">
+      <c r="E24" s="202"/>
+      <c r="F24" s="203">
         <v>1</v>
       </c>
-      <c r="G24" s="145">
+      <c r="G24" s="152">
         <v>1</v>
       </c>
       <c r="H24" s="22"/>
@@ -9835,29 +9868,29 @@
       <c r="H26" s="22"/>
       <c r="I26" s="57"/>
       <c r="J26" s="57"/>
-      <c r="K26" s="158" t="s">
+      <c r="K26" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="158"/>
-      <c r="M26" s="158"/>
-      <c r="N26" s="159"/>
+      <c r="L26" s="165"/>
+      <c r="M26" s="165"/>
+      <c r="N26" s="166"/>
       <c r="T26" s="25"/>
       <c r="U26" s="54"/>
       <c r="V26" s="54"/>
-      <c r="W26" s="175"/>
-      <c r="X26" s="175"/>
-      <c r="Y26" s="175"/>
+      <c r="W26" s="182"/>
+      <c r="X26" s="182"/>
+      <c r="Y26" s="182"/>
       <c r="Z26" s="25"/>
       <c r="AA26" s="25"/>
       <c r="AB26" s="25"/>
     </row>
     <row r="27" spans="2:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
-      <c r="C27" s="161" t="s">
+      <c r="C27" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="161"/>
-      <c r="E27" s="161"/>
+      <c r="D27" s="168"/>
+      <c r="E27" s="168"/>
       <c r="F27" s="71"/>
       <c r="G27" s="71"/>
       <c r="H27" s="22"/>
@@ -9879,13 +9912,13 @@
     </row>
     <row r="28" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="21"/>
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="131" t="s">
+      <c r="D28" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="118" t="s">
+      <c r="E28" s="119" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="71"/>
@@ -9909,13 +9942,13 @@
     </row>
     <row r="29" spans="2:28" ht="18" x14ac:dyDescent="0.25">
       <c r="B29" s="21"/>
-      <c r="C29" s="192">
+      <c r="C29" s="195">
         <v>0</v>
       </c>
-      <c r="D29" s="138" t="s">
+      <c r="D29" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="193">
+      <c r="E29" s="196">
         <v>0</v>
       </c>
       <c r="F29" s="34"/>
@@ -9939,32 +9972,32 @@
     </row>
     <row r="30" spans="2:28" ht="18" x14ac:dyDescent="0.25">
       <c r="B30" s="21"/>
-      <c r="C30" s="132">
+      <c r="C30" s="139">
         <v>1</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E30" s="133">
+      <c r="E30" s="140">
         <v>1</v>
       </c>
       <c r="F30" s="72"/>
       <c r="G30" s="72"/>
       <c r="H30" s="22"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="129" t="s">
+      <c r="J30" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="K30" s="130"/>
+      <c r="K30" s="137"/>
       <c r="L30" s="108"/>
       <c r="M30" s="104"/>
       <c r="N30" s="22"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B31" s="21"/>
-      <c r="C31" s="194"/>
+      <c r="C31" s="197"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="195"/>
+      <c r="E31" s="198"/>
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
       <c r="H31" s="22"/>
@@ -9977,26 +10010,26 @@
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B32" s="21"/>
-      <c r="C32" s="194"/>
+      <c r="C32" s="197"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="195"/>
+      <c r="E32" s="198"/>
       <c r="F32" s="34"/>
       <c r="G32" s="34"/>
       <c r="H32" s="22"/>
       <c r="I32" s="21"/>
       <c r="J32" s="106"/>
-      <c r="K32" s="176" t="s">
+      <c r="K32" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="177"/>
+      <c r="L32" s="184"/>
       <c r="M32" s="107"/>
       <c r="N32" s="22"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="21"/>
-      <c r="C33" s="194"/>
+      <c r="C33" s="197"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="195"/>
+      <c r="E33" s="198"/>
       <c r="F33" s="34"/>
       <c r="G33" s="34"/>
       <c r="H33" s="22"/>
@@ -10009,30 +10042,30 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="21"/>
-      <c r="C34" s="194"/>
+      <c r="C34" s="197"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="195"/>
+      <c r="E34" s="198"/>
       <c r="F34" s="34"/>
       <c r="G34" s="34"/>
       <c r="H34" s="22"/>
       <c r="I34" s="21"/>
       <c r="J34" s="106"/>
-      <c r="K34" s="176" t="s">
+      <c r="K34" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="177"/>
+      <c r="L34" s="184"/>
       <c r="M34" s="107"/>
       <c r="N34" s="22"/>
     </row>
     <row r="35" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="21"/>
-      <c r="C35" s="196" t="s">
+      <c r="C35" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="143" t="s">
+      <c r="D35" s="150" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="197" t="s">
+      <c r="E35" s="200" t="s">
         <v>1</v>
       </c>
       <c r="F35" s="34"/>
@@ -10055,7 +10088,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="21"/>
       <c r="J36" s="106"/>
-      <c r="K36" s="118" t="s">
+      <c r="K36" s="119" t="s">
         <v>62</v>
       </c>
       <c r="L36" s="25"/>
@@ -10071,12 +10104,12 @@
       <c r="G37" s="25"/>
       <c r="H37" s="22"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="186"/>
-      <c r="K37" s="119" t="s">
+      <c r="J37" s="189"/>
+      <c r="K37" s="120" t="s">
         <v>1</v>
       </c>
       <c r="L37" s="72"/>
-      <c r="M37" s="187"/>
+      <c r="M37" s="190"/>
       <c r="N37" s="22"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -10088,10 +10121,10 @@
       <c r="G38" s="25"/>
       <c r="H38" s="22"/>
       <c r="I38" s="21"/>
-      <c r="J38" s="188"/>
-      <c r="K38" s="189"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="191"/>
+      <c r="J38" s="191"/>
+      <c r="K38" s="192"/>
+      <c r="L38" s="193"/>
+      <c r="M38" s="194"/>
       <c r="N38" s="22"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -10128,20 +10161,20 @@
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
-      <c r="E41" s="162" t="s">
+      <c r="E41" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="162"/>
-      <c r="G41" s="162"/>
-      <c r="H41" s="163"/>
+      <c r="F41" s="169"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="170"/>
       <c r="I41" s="26"/>
       <c r="J41" s="28"/>
-      <c r="K41" s="162" t="s">
+      <c r="K41" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="L41" s="162"/>
-      <c r="M41" s="162"/>
-      <c r="N41" s="163"/>
+      <c r="L41" s="169"/>
+      <c r="M41" s="169"/>
+      <c r="N41" s="170"/>
     </row>
     <row r="42" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10173,8 +10206,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:N26"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10250,27 +10283,27 @@
     </row>
     <row r="5" spans="2:27" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
-      <c r="C5" s="160" t="s">
+      <c r="C5" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
       <c r="F5" s="99"/>
       <c r="G5" s="99"/>
       <c r="H5" s="20"/>
       <c r="I5" s="55"/>
-      <c r="J5" s="174" t="s">
+      <c r="J5" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
       <c r="M5" s="109"/>
       <c r="N5" s="47"/>
       <c r="U5" s="111"/>
       <c r="V5" s="55"/>
-      <c r="W5" s="180"/>
-      <c r="X5" s="180"/>
-      <c r="Y5" s="180"/>
+      <c r="W5" s="187"/>
+      <c r="X5" s="187"/>
+      <c r="Y5" s="187"/>
       <c r="Z5" s="55"/>
       <c r="AA5" s="111"/>
     </row>
@@ -10321,10 +10354,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="85"/>
-      <c r="F7" s="201">
+      <c r="F7" s="204">
         <v>0</v>
       </c>
-      <c r="G7" s="201">
+      <c r="G7" s="204">
         <v>1</v>
       </c>
       <c r="H7" s="30"/>
@@ -10335,8 +10368,8 @@
       <c r="K7" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="203"/>
-      <c r="M7" s="185"/>
+      <c r="L7" s="206"/>
+      <c r="M7" s="188"/>
       <c r="N7" s="50"/>
       <c r="U7" s="25"/>
       <c r="V7" s="102"/>
@@ -10374,7 +10407,7 @@
       <c r="L8" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="116"/>
+      <c r="M8" s="117"/>
       <c r="N8" s="50"/>
       <c r="U8" s="25"/>
       <c r="V8" s="102"/>
@@ -10389,14 +10422,14 @@
       <c r="C9" s="86"/>
       <c r="D9" s="91"/>
       <c r="E9" s="91"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="202"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
       <c r="H9" s="30"/>
       <c r="I9" s="62"/>
       <c r="J9" s="78"/>
       <c r="K9" s="79"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="185"/>
+      <c r="L9" s="207"/>
+      <c r="M9" s="188"/>
       <c r="N9" s="50"/>
       <c r="U9" s="25"/>
       <c r="V9" s="102"/>
@@ -10417,8 +10450,8 @@
       <c r="I10" s="62"/>
       <c r="J10" s="52"/>
       <c r="K10" s="53"/>
-      <c r="L10" s="205"/>
-      <c r="M10" s="185"/>
+      <c r="L10" s="208"/>
+      <c r="M10" s="188"/>
       <c r="N10" s="50"/>
       <c r="U10" s="25"/>
       <c r="V10" s="102"/>
@@ -10439,8 +10472,8 @@
       <c r="I11" s="62"/>
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
-      <c r="L11" s="205"/>
-      <c r="M11" s="185"/>
+      <c r="L11" s="208"/>
+      <c r="M11" s="188"/>
       <c r="N11" s="50"/>
       <c r="U11" s="25"/>
       <c r="V11" s="102"/>
@@ -10461,8 +10494,8 @@
       <c r="I12" s="62"/>
       <c r="J12" s="52"/>
       <c r="K12" s="53"/>
-      <c r="L12" s="205"/>
-      <c r="M12" s="185"/>
+      <c r="L12" s="208"/>
+      <c r="M12" s="188"/>
       <c r="N12" s="50"/>
       <c r="U12" s="25"/>
       <c r="V12" s="102"/>
@@ -10495,8 +10528,8 @@
       <c r="K13" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="205"/>
-      <c r="M13" s="185"/>
+      <c r="L13" s="208"/>
+      <c r="M13" s="188"/>
       <c r="N13" s="50"/>
       <c r="U13" s="25"/>
       <c r="V13" s="102"/>
@@ -10654,7 +10687,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="22"/>
-      <c r="I20" s="54"/>
+      <c r="I20" s="102"/>
       <c r="J20" s="102"/>
       <c r="K20" s="102"/>
       <c r="L20" s="102"/>
@@ -10676,17 +10709,17 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="22"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="178"/>
-      <c r="K21" s="178"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="185"/>
+      <c r="K21" s="185"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
       <c r="N21" s="50"/>
       <c r="U21" s="25"/>
       <c r="V21" s="54"/>
-      <c r="W21" s="178"/>
-      <c r="X21" s="178"/>
-      <c r="Y21" s="113"/>
+      <c r="W21" s="185"/>
+      <c r="X21" s="185"/>
+      <c r="Y21" s="114"/>
       <c r="Z21" s="54"/>
       <c r="AA21" s="25"/>
     </row>
@@ -10698,16 +10731,16 @@
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="22"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="114"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="186"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
       <c r="N22" s="50"/>
       <c r="U22" s="25"/>
       <c r="V22" s="54"/>
-      <c r="W22" s="179"/>
-      <c r="X22" s="179"/>
+      <c r="W22" s="186"/>
+      <c r="X22" s="186"/>
       <c r="Y22" s="96"/>
       <c r="Z22" s="54"/>
       <c r="AA22" s="25"/>
@@ -10720,16 +10753,16 @@
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="22"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="114"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="186"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
       <c r="N23" s="50"/>
       <c r="U23" s="25"/>
       <c r="V23" s="54"/>
-      <c r="W23" s="179"/>
-      <c r="X23" s="179"/>
+      <c r="W23" s="186"/>
+      <c r="X23" s="186"/>
       <c r="Y23" s="96"/>
       <c r="Z23" s="54"/>
       <c r="AA23" s="25"/>
@@ -10750,17 +10783,17 @@
         <v>1</v>
       </c>
       <c r="H24" s="22"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="114"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="115"/>
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
       <c r="M24" s="94"/>
       <c r="N24" s="50"/>
       <c r="U24" s="25"/>
       <c r="V24" s="54"/>
-      <c r="W24" s="115"/>
-      <c r="X24" s="116"/>
-      <c r="Y24" s="116"/>
+      <c r="W24" s="116"/>
+      <c r="X24" s="117"/>
+      <c r="Y24" s="117"/>
       <c r="Z24" s="54"/>
       <c r="AA24" s="25"/>
     </row>
@@ -10796,27 +10829,27 @@
       <c r="H26" s="22"/>
       <c r="I26" s="57"/>
       <c r="J26" s="57"/>
-      <c r="K26" s="158" t="s">
+      <c r="K26" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="158"/>
-      <c r="M26" s="158"/>
-      <c r="N26" s="159"/>
+      <c r="L26" s="165"/>
+      <c r="M26" s="165"/>
+      <c r="N26" s="166"/>
       <c r="U26" s="25"/>
       <c r="V26" s="54"/>
       <c r="W26" s="102"/>
-      <c r="X26" s="117"/>
-      <c r="Y26" s="117"/>
-      <c r="Z26" s="112"/>
+      <c r="X26" s="118"/>
+      <c r="Y26" s="118"/>
+      <c r="Z26" s="113"/>
       <c r="AA26" s="25"/>
     </row>
     <row r="27" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
-      <c r="C27" s="161" t="s">
+      <c r="C27" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="161"/>
-      <c r="E27" s="161"/>
+      <c r="D27" s="168"/>
+      <c r="E27" s="168"/>
       <c r="F27" s="71"/>
       <c r="G27" s="71"/>
       <c r="H27" s="22"/>
@@ -10905,12 +10938,12 @@
       <c r="G30" s="72"/>
       <c r="H30" s="22"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="126" t="s">
+      <c r="J30" s="265" t="s">
         <v>49</v>
       </c>
-      <c r="K30" s="127"/>
-      <c r="L30" s="120"/>
-      <c r="M30" s="121"/>
+      <c r="K30" s="266"/>
+      <c r="L30" s="266"/>
+      <c r="M30" s="267"/>
       <c r="N30" s="22"/>
       <c r="U30" s="25"/>
       <c r="V30" s="25"/>
@@ -10929,10 +10962,10 @@
       <c r="G31" s="34"/>
       <c r="H31" s="22"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="122"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="123"/>
+      <c r="J31" s="268"/>
+      <c r="K31" s="269"/>
+      <c r="L31" s="269"/>
+      <c r="M31" s="270"/>
       <c r="N31" s="22"/>
       <c r="U31" s="25"/>
       <c r="V31" s="25"/>
@@ -10951,12 +10984,12 @@
       <c r="G32" s="34"/>
       <c r="H32" s="22"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="124"/>
-      <c r="K32" s="176" t="s">
+      <c r="J32" s="268"/>
+      <c r="K32" s="261" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="177"/>
-      <c r="M32" s="125"/>
+      <c r="L32" s="262"/>
+      <c r="M32" s="270"/>
       <c r="N32" s="22"/>
       <c r="U32" s="25"/>
       <c r="V32" s="25"/>
@@ -10975,10 +11008,10 @@
       <c r="G33" s="34"/>
       <c r="H33" s="22"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="124"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="125"/>
+      <c r="J33" s="268"/>
+      <c r="K33" s="269"/>
+      <c r="L33" s="269"/>
+      <c r="M33" s="270"/>
       <c r="N33" s="22"/>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
@@ -10990,12 +11023,12 @@
       <c r="G34" s="34"/>
       <c r="H34" s="22"/>
       <c r="I34" s="21"/>
-      <c r="J34" s="124"/>
-      <c r="K34" s="176" t="s">
+      <c r="J34" s="268"/>
+      <c r="K34" s="261" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="177"/>
-      <c r="M34" s="125"/>
+      <c r="L34" s="262"/>
+      <c r="M34" s="270"/>
       <c r="N34" s="22"/>
       <c r="U34" s="7"/>
     </row>
@@ -11014,10 +11047,10 @@
       <c r="G35" s="34"/>
       <c r="H35" s="22"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="124"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="125"/>
+      <c r="J35" s="268"/>
+      <c r="K35" s="269"/>
+      <c r="L35" s="269"/>
+      <c r="M35" s="270"/>
       <c r="N35" s="22"/>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
@@ -11029,12 +11062,12 @@
       <c r="G36" s="25"/>
       <c r="H36" s="22"/>
       <c r="I36" s="21"/>
-      <c r="J36" s="124"/>
-      <c r="K36" s="13" t="s">
+      <c r="J36" s="268"/>
+      <c r="K36" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="L36" s="25"/>
-      <c r="M36" s="125"/>
+      <c r="L36" s="269"/>
+      <c r="M36" s="270"/>
       <c r="N36" s="22"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
@@ -11046,12 +11079,12 @@
       <c r="G37" s="25"/>
       <c r="H37" s="22"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="206"/>
+      <c r="J37" s="127"/>
       <c r="K37" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="L37" s="72"/>
-      <c r="M37" s="207"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="128"/>
       <c r="N37" s="22"/>
     </row>
     <row r="38" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11063,10 +11096,10 @@
       <c r="G38" s="25"/>
       <c r="H38" s="22"/>
       <c r="I38" s="21"/>
-      <c r="J38" s="208"/>
-      <c r="K38" s="209"/>
-      <c r="L38" s="210"/>
-      <c r="M38" s="211"/>
+      <c r="J38" s="129"/>
+      <c r="K38" s="130"/>
+      <c r="L38" s="131"/>
+      <c r="M38" s="132"/>
       <c r="N38" s="22"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
@@ -11103,24 +11136,24 @@
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
-      <c r="E41" s="162" t="s">
+      <c r="E41" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="162"/>
-      <c r="G41" s="162"/>
-      <c r="H41" s="163"/>
+      <c r="F41" s="169"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="170"/>
       <c r="I41" s="26"/>
       <c r="J41" s="28"/>
-      <c r="K41" s="162" t="s">
+      <c r="K41" s="169" t="s">
         <v>19</v>
       </c>
-      <c r="L41" s="162"/>
-      <c r="M41" s="162"/>
-      <c r="N41" s="163"/>
+      <c r="L41" s="169"/>
+      <c r="M41" s="169"/>
+      <c r="N41" s="170"/>
     </row>
     <row r="42" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="W21:X21"/>
@@ -11130,7 +11163,6 @@
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:J23"/>
     <mergeCell ref="K22:K23"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K32:L32"/>
@@ -11147,30 +11179,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="212"/>
-    <col min="3" max="3" width="13.85546875" style="214" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="212" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="212" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="214" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="212" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="212"/>
-    <col min="10" max="10" width="14.7109375" style="212" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" style="212" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="212" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="212" customWidth="1"/>
-    <col min="14" max="14" width="6" style="212" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="212" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="212"/>
+    <col min="1" max="2" width="9.140625" style="215"/>
+    <col min="3" max="3" width="13.85546875" style="217" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="215" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="215" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="217" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="215" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="215"/>
+    <col min="10" max="10" width="14.7109375" style="215" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="215" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="215" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="215" customWidth="1"/>
+    <col min="14" max="14" width="6" style="215" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="215" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="215"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="213" t="s">
+      <c r="C2" s="216" t="s">
         <v>60</v>
       </c>
       <c r="K2" s="10"/>
@@ -11180,38 +11212,38 @@
     </row>
     <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="215"/>
-      <c r="C4" s="216"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="216"/>
-      <c r="G4" s="217"/>
-      <c r="H4" s="218"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
-      <c r="K4" s="219"/>
-      <c r="L4" s="219"/>
-      <c r="M4" s="219"/>
-      <c r="N4" s="220"/>
-    </row>
-    <row r="5" spans="2:19" s="228" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="221"/>
-      <c r="C5" s="222" t="s">
+      <c r="B4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="220"/>
+      <c r="E4" s="220"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="221"/>
+      <c r="I4" s="222"/>
+      <c r="J4" s="222"/>
+      <c r="K4" s="222"/>
+      <c r="L4" s="222"/>
+      <c r="M4" s="222"/>
+      <c r="N4" s="223"/>
+    </row>
+    <row r="5" spans="2:19" s="231" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="224"/>
+      <c r="C5" s="225" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="223"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="225"/>
-      <c r="J5" s="226" t="s">
+      <c r="D5" s="225"/>
+      <c r="E5" s="225"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="227"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="226"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="227"/>
+      <c r="K5" s="229"/>
+      <c r="L5" s="229"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="230"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="33"/>
@@ -11232,17 +11264,17 @@
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="102"/>
-      <c r="J6" s="229" t="s">
+      <c r="J6" s="232" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="229" t="s">
+      <c r="K6" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="229" t="s">
+      <c r="L6" s="232" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="113"/>
-      <c r="N6" s="230"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="233"/>
     </row>
     <row r="7" spans="2:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="33"/>
@@ -11256,7 +11288,7 @@
       <c r="F7" s="84">
         <v>0</v>
       </c>
-      <c r="G7" s="201">
+      <c r="G7" s="204">
         <v>1</v>
       </c>
       <c r="H7" s="30"/>
@@ -11267,19 +11299,19 @@
       <c r="K7" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="203"/>
-      <c r="M7" s="185"/>
-      <c r="N7" s="230"/>
+      <c r="L7" s="206"/>
+      <c r="M7" s="188"/>
+      <c r="N7" s="233"/>
     </row>
     <row r="8" spans="2:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="33"/>
-      <c r="C8" s="246">
+      <c r="C8" s="247">
         <v>1</v>
       </c>
-      <c r="D8" s="247" t="s">
+      <c r="D8" s="248" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="247" t="s">
+      <c r="E8" s="248" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="110" t="s">
@@ -11290,15 +11322,15 @@
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="102"/>
-      <c r="J8" s="231">
+      <c r="J8" s="234">
         <v>1</v>
       </c>
-      <c r="K8" s="232" t="s">
+      <c r="K8" s="235" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="233"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="230"/>
+      <c r="L8" s="236"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="233"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="33"/>
@@ -11306,15 +11338,15 @@
       <c r="D9" s="91"/>
       <c r="E9" s="91"/>
       <c r="F9" s="86"/>
-      <c r="G9" s="202"/>
+      <c r="G9" s="205"/>
       <c r="H9" s="30"/>
       <c r="I9" s="62"/>
       <c r="J9" s="78"/>
       <c r="K9" s="79"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="185"/>
-      <c r="N9" s="230"/>
-      <c r="S9" s="234"/>
+      <c r="L9" s="207"/>
+      <c r="M9" s="188"/>
+      <c r="N9" s="233"/>
+      <c r="S9" s="237"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
@@ -11327,9 +11359,9 @@
       <c r="I10" s="62"/>
       <c r="J10" s="52"/>
       <c r="K10" s="53"/>
-      <c r="L10" s="205"/>
-      <c r="M10" s="185"/>
-      <c r="N10" s="230"/>
+      <c r="L10" s="208"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="233"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
@@ -11342,9 +11374,9 @@
       <c r="I11" s="62"/>
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
-      <c r="L11" s="205"/>
-      <c r="M11" s="185"/>
-      <c r="N11" s="230"/>
+      <c r="L11" s="208"/>
+      <c r="M11" s="188"/>
+      <c r="N11" s="233"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="33"/>
@@ -11357,9 +11389,9 @@
       <c r="I12" s="62"/>
       <c r="J12" s="52"/>
       <c r="K12" s="53"/>
-      <c r="L12" s="205"/>
-      <c r="M12" s="185"/>
-      <c r="N12" s="230"/>
+      <c r="L12" s="208"/>
+      <c r="M12" s="188"/>
+      <c r="N12" s="233"/>
     </row>
     <row r="13" spans="2:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="33"/>
@@ -11373,7 +11405,7 @@
       <c r="F13" s="84">
         <v>0</v>
       </c>
-      <c r="G13" s="201">
+      <c r="G13" s="204">
         <v>1</v>
       </c>
       <c r="H13" s="30"/>
@@ -11384,9 +11416,9 @@
       <c r="K13" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="205"/>
-      <c r="M13" s="185"/>
-      <c r="N13" s="230"/>
+      <c r="L13" s="208"/>
+      <c r="M13" s="188"/>
+      <c r="N13" s="233"/>
     </row>
     <row r="14" spans="2:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="33"/>
@@ -11396,8 +11428,8 @@
       <c r="D14" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="247"/>
-      <c r="F14" s="248" t="s">
+      <c r="E14" s="248"/>
+      <c r="F14" s="249" t="s">
         <v>56</v>
       </c>
       <c r="G14" s="90">
@@ -11409,7 +11441,7 @@
       <c r="K14" s="102"/>
       <c r="L14" s="102"/>
       <c r="M14" s="102"/>
-      <c r="N14" s="230"/>
+      <c r="N14" s="233"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="33"/>
@@ -11419,14 +11451,14 @@
       <c r="F15" s="86">
         <v>1</v>
       </c>
-      <c r="G15" s="202"/>
+      <c r="G15" s="205"/>
       <c r="H15" s="32"/>
       <c r="I15" s="102"/>
-      <c r="J15" s="225"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="225"/>
-      <c r="M15" s="225"/>
-      <c r="N15" s="230"/>
+      <c r="J15" s="228"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="228"/>
+      <c r="M15" s="228"/>
+      <c r="N15" s="233"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="33"/>
@@ -11443,7 +11475,7 @@
       <c r="K16" s="102"/>
       <c r="L16" s="102"/>
       <c r="M16" s="102"/>
-      <c r="N16" s="230"/>
+      <c r="N16" s="233"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
@@ -11460,7 +11492,7 @@
       <c r="K17" s="102"/>
       <c r="L17" s="102"/>
       <c r="M17" s="102"/>
-      <c r="N17" s="230"/>
+      <c r="N17" s="233"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
@@ -11477,7 +11509,7 @@
       <c r="K18" s="102"/>
       <c r="L18" s="102"/>
       <c r="M18" s="102"/>
-      <c r="N18" s="230"/>
+      <c r="N18" s="233"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
@@ -11494,7 +11526,7 @@
       <c r="K19" s="102"/>
       <c r="L19" s="102"/>
       <c r="M19" s="102"/>
-      <c r="N19" s="230"/>
+      <c r="N19" s="233"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
@@ -11511,7 +11543,7 @@
       <c r="K20" s="102"/>
       <c r="L20" s="102"/>
       <c r="M20" s="102"/>
-      <c r="N20" s="230"/>
+      <c r="N20" s="233"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="33"/>
@@ -11524,11 +11556,11 @@
       <c r="G21" s="14"/>
       <c r="H21" s="32"/>
       <c r="I21" s="102"/>
-      <c r="J21" s="178"/>
-      <c r="K21" s="178"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="230"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="233"/>
     </row>
     <row r="22" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
@@ -11541,11 +11573,11 @@
       <c r="G22" s="14"/>
       <c r="H22" s="32"/>
       <c r="I22" s="102"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="230"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="233"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
@@ -11558,11 +11590,11 @@
       <c r="G23" s="14"/>
       <c r="H23" s="32"/>
       <c r="I23" s="102"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="230"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="233"/>
     </row>
     <row r="24" spans="2:21" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
@@ -11581,11 +11613,11 @@
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="102"/>
-      <c r="J24" s="114"/>
+      <c r="J24" s="115"/>
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
       <c r="M24" s="94"/>
-      <c r="N24" s="230"/>
+      <c r="N24" s="233"/>
       <c r="U24" s="8"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
@@ -11601,7 +11633,7 @@
       <c r="K25" s="102"/>
       <c r="L25" s="102"/>
       <c r="M25" s="102"/>
-      <c r="N25" s="230"/>
+      <c r="N25" s="233"/>
     </row>
     <row r="26" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="33"/>
@@ -11611,31 +11643,31 @@
       <c r="F26" s="34"/>
       <c r="G26" s="10"/>
       <c r="H26" s="32"/>
-      <c r="I26" s="235"/>
-      <c r="J26" s="235"/>
-      <c r="K26" s="236" t="s">
+      <c r="I26" s="238"/>
+      <c r="J26" s="238"/>
+      <c r="K26" s="239" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="236"/>
-      <c r="M26" s="236"/>
-      <c r="N26" s="237"/>
+      <c r="L26" s="239"/>
+      <c r="M26" s="239"/>
+      <c r="N26" s="240"/>
     </row>
     <row r="27" spans="2:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="33"/>
-      <c r="C27" s="238" t="s">
+      <c r="C27" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
+      <c r="D27" s="241"/>
+      <c r="E27" s="241"/>
       <c r="F27" s="72"/>
       <c r="G27" s="72"/>
       <c r="H27" s="32"/>
-      <c r="I27" s="215"/>
-      <c r="J27" s="217"/>
-      <c r="K27" s="217"/>
-      <c r="L27" s="217"/>
-      <c r="M27" s="217"/>
-      <c r="N27" s="218"/>
+      <c r="I27" s="218"/>
+      <c r="J27" s="220"/>
+      <c r="K27" s="220"/>
+      <c r="L27" s="220"/>
+      <c r="M27" s="220"/>
+      <c r="N27" s="221"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
@@ -11684,7 +11716,7 @@
       <c r="C30" s="37">
         <v>1</v>
       </c>
-      <c r="D30" s="232" t="s">
+      <c r="D30" s="235" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="37">
@@ -11695,7 +11727,7 @@
       <c r="H30" s="32"/>
       <c r="I30" s="33"/>
       <c r="J30" s="103"/>
-      <c r="K30" s="128" t="s">
+      <c r="K30" s="135" t="s">
         <v>49</v>
       </c>
       <c r="L30" s="108"/>
@@ -11727,10 +11759,10 @@
       <c r="H32" s="32"/>
       <c r="I32" s="33"/>
       <c r="J32" s="100"/>
-      <c r="K32" s="249" t="s">
+      <c r="K32" s="263" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="250"/>
+      <c r="L32" s="264"/>
       <c r="M32" s="105"/>
       <c r="N32" s="32"/>
     </row>
@@ -11759,10 +11791,10 @@
       <c r="H34" s="32"/>
       <c r="I34" s="33"/>
       <c r="J34" s="100"/>
-      <c r="K34" s="239" t="s">
+      <c r="K34" s="261" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="240"/>
+      <c r="L34" s="262"/>
       <c r="M34" s="105"/>
       <c r="N34" s="32"/>
     </row>
@@ -11797,7 +11829,7 @@
       <c r="H36" s="32"/>
       <c r="I36" s="33"/>
       <c r="J36" s="100"/>
-      <c r="K36" s="201" t="s">
+      <c r="K36" s="204" t="s">
         <v>62</v>
       </c>
       <c r="L36" s="10"/>
@@ -11813,12 +11845,12 @@
       <c r="G37" s="10"/>
       <c r="H37" s="32"/>
       <c r="I37" s="33"/>
-      <c r="J37" s="186"/>
-      <c r="K37" s="119" t="s">
+      <c r="J37" s="189"/>
+      <c r="K37" s="120" t="s">
         <v>63</v>
       </c>
       <c r="L37" s="72"/>
-      <c r="M37" s="187"/>
+      <c r="M37" s="190"/>
       <c r="N37" s="32"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -11830,10 +11862,10 @@
       <c r="G38" s="10"/>
       <c r="H38" s="32"/>
       <c r="I38" s="33"/>
-      <c r="J38" s="188"/>
-      <c r="K38" s="189"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="191"/>
+      <c r="J38" s="191"/>
+      <c r="K38" s="192"/>
+      <c r="L38" s="193"/>
+      <c r="M38" s="194"/>
       <c r="N38" s="32"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -11867,33 +11899,30 @@
       <c r="N40" s="32"/>
     </row>
     <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="241"/>
-      <c r="C41" s="242"/>
-      <c r="D41" s="243"/>
-      <c r="E41" s="244" t="s">
+      <c r="B41" s="242"/>
+      <c r="C41" s="243"/>
+      <c r="D41" s="244"/>
+      <c r="E41" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="244"/>
-      <c r="G41" s="244"/>
-      <c r="H41" s="245"/>
-      <c r="I41" s="241"/>
-      <c r="J41" s="243"/>
-      <c r="K41" s="244" t="s">
+      <c r="F41" s="245"/>
+      <c r="G41" s="245"/>
+      <c r="H41" s="246"/>
+      <c r="I41" s="242"/>
+      <c r="J41" s="244"/>
+      <c r="K41" s="245" t="s">
         <v>19</v>
       </c>
-      <c r="L41" s="244"/>
-      <c r="M41" s="244"/>
-      <c r="N41" s="245"/>
+      <c r="L41" s="245"/>
+      <c r="M41" s="245"/>
+      <c r="N41" s="246"/>
     </row>
     <row r="42" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="8">
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="K41:N41"/>
@@ -11911,31 +11940,31 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:T42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="212"/>
-    <col min="3" max="3" width="13.85546875" style="214" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="212" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="212" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="214" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" style="212" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="212"/>
-    <col min="10" max="10" width="14.7109375" style="212" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" style="212" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="212" customWidth="1"/>
-    <col min="13" max="13" width="6" style="212" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="212" customWidth="1"/>
-    <col min="15" max="20" width="9.140625" style="212"/>
-    <col min="21" max="21" width="22.7109375" style="212" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="212"/>
+    <col min="1" max="2" width="9.140625" style="215"/>
+    <col min="3" max="3" width="13.85546875" style="217" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="215" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="215" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="217" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="215" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="215"/>
+    <col min="10" max="10" width="14.7109375" style="215" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="215" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="215" customWidth="1"/>
+    <col min="13" max="13" width="6" style="215" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="215" customWidth="1"/>
+    <col min="15" max="20" width="9.140625" style="215"/>
+    <col min="21" max="21" width="22.7109375" style="215" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="215"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="213" t="s">
+      <c r="C2" s="216" t="s">
         <v>23</v>
       </c>
       <c r="K2" s="10"/>
@@ -11944,38 +11973,38 @@
     </row>
     <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="215"/>
-      <c r="C4" s="216"/>
-      <c r="D4" s="217"/>
-      <c r="E4" s="217"/>
-      <c r="F4" s="216"/>
-      <c r="G4" s="217"/>
-      <c r="H4" s="218"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
-      <c r="K4" s="219"/>
-      <c r="L4" s="219"/>
-      <c r="M4" s="219"/>
-      <c r="N4" s="220"/>
-    </row>
-    <row r="5" spans="2:18" s="228" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="221"/>
-      <c r="C5" s="222" t="s">
+      <c r="B4" s="218"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="220"/>
+      <c r="E4" s="220"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="220"/>
+      <c r="H4" s="221"/>
+      <c r="I4" s="222"/>
+      <c r="J4" s="222"/>
+      <c r="K4" s="222"/>
+      <c r="L4" s="222"/>
+      <c r="M4" s="222"/>
+      <c r="N4" s="223"/>
+    </row>
+    <row r="5" spans="2:18" s="231" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="224"/>
+      <c r="C5" s="225" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="223"/>
-      <c r="G5" s="223"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="225"/>
-      <c r="J5" s="226" t="s">
+      <c r="D5" s="225"/>
+      <c r="E5" s="225"/>
+      <c r="F5" s="226"/>
+      <c r="G5" s="226"/>
+      <c r="H5" s="227"/>
+      <c r="I5" s="228"/>
+      <c r="J5" s="229" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="226"/>
-      <c r="L5" s="226"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="227"/>
+      <c r="K5" s="229"/>
+      <c r="L5" s="229"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="230"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="33"/>
@@ -11996,17 +12025,17 @@
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="102"/>
-      <c r="J6" s="229" t="s">
+      <c r="J6" s="232" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="229" t="s">
+      <c r="K6" s="232" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="229" t="s">
+      <c r="L6" s="232" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="113"/>
-      <c r="N6" s="230"/>
+      <c r="M6" s="114"/>
+      <c r="N6" s="233"/>
     </row>
     <row r="7" spans="2:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="33"/>
@@ -12020,7 +12049,7 @@
       <c r="F7" s="84">
         <v>0</v>
       </c>
-      <c r="G7" s="251">
+      <c r="G7" s="250">
         <v>1</v>
       </c>
       <c r="H7" s="30"/>
@@ -12031,9 +12060,9 @@
       <c r="K7" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="203"/>
-      <c r="M7" s="185"/>
-      <c r="N7" s="230"/>
+      <c r="L7" s="206"/>
+      <c r="M7" s="188"/>
+      <c r="N7" s="233"/>
     </row>
     <row r="8" spans="2:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="33"/>
@@ -12061,8 +12090,8 @@
         <v>42</v>
       </c>
       <c r="L8" s="80"/>
-      <c r="M8" s="116"/>
-      <c r="N8" s="230"/>
+      <c r="M8" s="117"/>
+      <c r="N8" s="233"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="33"/>
@@ -12070,15 +12099,15 @@
       <c r="D9" s="91"/>
       <c r="E9" s="91"/>
       <c r="F9" s="86"/>
-      <c r="G9" s="252"/>
+      <c r="G9" s="251"/>
       <c r="H9" s="30"/>
       <c r="I9" s="62"/>
       <c r="J9" s="78"/>
       <c r="K9" s="79"/>
-      <c r="L9" s="204"/>
-      <c r="M9" s="185"/>
-      <c r="N9" s="230"/>
-      <c r="R9" s="234"/>
+      <c r="L9" s="207"/>
+      <c r="M9" s="188"/>
+      <c r="N9" s="233"/>
+      <c r="R9" s="237"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
@@ -12091,9 +12120,9 @@
       <c r="I10" s="62"/>
       <c r="J10" s="52"/>
       <c r="K10" s="53"/>
-      <c r="L10" s="205"/>
-      <c r="M10" s="185"/>
-      <c r="N10" s="230"/>
+      <c r="L10" s="208"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="233"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
@@ -12106,9 +12135,9 @@
       <c r="I11" s="62"/>
       <c r="J11" s="52"/>
       <c r="K11" s="53"/>
-      <c r="L11" s="205"/>
-      <c r="M11" s="185"/>
-      <c r="N11" s="230"/>
+      <c r="L11" s="208"/>
+      <c r="M11" s="188"/>
+      <c r="N11" s="233"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="33"/>
@@ -12121,9 +12150,9 @@
       <c r="I12" s="62"/>
       <c r="J12" s="52"/>
       <c r="K12" s="53"/>
-      <c r="L12" s="205"/>
-      <c r="M12" s="185"/>
-      <c r="N12" s="230"/>
+      <c r="L12" s="208"/>
+      <c r="M12" s="188"/>
+      <c r="N12" s="233"/>
     </row>
     <row r="13" spans="2:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="33"/>
@@ -12137,7 +12166,7 @@
       <c r="F13" s="84">
         <v>0</v>
       </c>
-      <c r="G13" s="251">
+      <c r="G13" s="250">
         <v>1</v>
       </c>
       <c r="H13" s="30"/>
@@ -12148,9 +12177,9 @@
       <c r="K13" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="205"/>
-      <c r="M13" s="185"/>
-      <c r="N13" s="230"/>
+      <c r="L13" s="208"/>
+      <c r="M13" s="188"/>
+      <c r="N13" s="233"/>
     </row>
     <row r="14" spans="2:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="33"/>
@@ -12160,11 +12189,11 @@
       <c r="D14" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="247"/>
-      <c r="F14" s="248">
+      <c r="E14" s="248"/>
+      <c r="F14" s="249">
         <v>0</v>
       </c>
-      <c r="G14" s="253">
+      <c r="G14" s="252">
         <v>1</v>
       </c>
       <c r="H14" s="32"/>
@@ -12173,7 +12202,7 @@
       <c r="K14" s="102"/>
       <c r="L14" s="102"/>
       <c r="M14" s="102"/>
-      <c r="N14" s="230"/>
+      <c r="N14" s="233"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="33"/>
@@ -12181,14 +12210,14 @@
       <c r="D15" s="91"/>
       <c r="E15" s="91"/>
       <c r="F15" s="86"/>
-      <c r="G15" s="252"/>
+      <c r="G15" s="251"/>
       <c r="H15" s="32"/>
       <c r="I15" s="102"/>
-      <c r="J15" s="225"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="225"/>
-      <c r="M15" s="225"/>
-      <c r="N15" s="230"/>
+      <c r="J15" s="228"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="228"/>
+      <c r="M15" s="228"/>
+      <c r="N15" s="233"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="33"/>
@@ -12203,7 +12232,7 @@
       <c r="K16" s="102"/>
       <c r="L16" s="102"/>
       <c r="M16" s="102"/>
-      <c r="N16" s="230"/>
+      <c r="N16" s="233"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
@@ -12218,7 +12247,7 @@
       <c r="K17" s="102"/>
       <c r="L17" s="102"/>
       <c r="M17" s="102"/>
-      <c r="N17" s="230"/>
+      <c r="N17" s="233"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
@@ -12233,7 +12262,7 @@
       <c r="K18" s="102"/>
       <c r="L18" s="102"/>
       <c r="M18" s="102"/>
-      <c r="N18" s="230"/>
+      <c r="N18" s="233"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
@@ -12248,7 +12277,7 @@
       <c r="K19" s="102"/>
       <c r="L19" s="102"/>
       <c r="M19" s="102"/>
-      <c r="N19" s="230"/>
+      <c r="N19" s="233"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
@@ -12263,7 +12292,7 @@
       <c r="K20" s="102"/>
       <c r="L20" s="102"/>
       <c r="M20" s="102"/>
-      <c r="N20" s="230"/>
+      <c r="N20" s="233"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="33"/>
@@ -12274,11 +12303,11 @@
       <c r="G21" s="37"/>
       <c r="H21" s="32"/>
       <c r="I21" s="102"/>
-      <c r="J21" s="178"/>
-      <c r="K21" s="178"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="113"/>
-      <c r="N21" s="230"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="233"/>
     </row>
     <row r="22" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
@@ -12289,11 +12318,11 @@
       <c r="G22" s="37"/>
       <c r="H22" s="32"/>
       <c r="I22" s="102"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="230"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="233"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
@@ -12304,11 +12333,11 @@
       <c r="G23" s="37"/>
       <c r="H23" s="32"/>
       <c r="I23" s="102"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="114"/>
-      <c r="N23" s="230"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="233"/>
     </row>
     <row r="24" spans="2:20" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
@@ -12327,11 +12356,11 @@
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="102"/>
-      <c r="J24" s="114"/>
+      <c r="J24" s="115"/>
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
       <c r="M24" s="94"/>
-      <c r="N24" s="230"/>
+      <c r="N24" s="233"/>
       <c r="T24" s="8"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
@@ -12347,7 +12376,7 @@
       <c r="K25" s="102"/>
       <c r="L25" s="102"/>
       <c r="M25" s="102"/>
-      <c r="N25" s="230"/>
+      <c r="N25" s="233"/>
     </row>
     <row r="26" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="33"/>
@@ -12357,31 +12386,31 @@
       <c r="F26" s="34"/>
       <c r="G26" s="10"/>
       <c r="H26" s="32"/>
-      <c r="I26" s="235"/>
-      <c r="J26" s="235"/>
-      <c r="K26" s="236" t="s">
+      <c r="I26" s="238"/>
+      <c r="J26" s="238"/>
+      <c r="K26" s="239" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="236"/>
-      <c r="M26" s="236"/>
-      <c r="N26" s="237"/>
+      <c r="L26" s="239"/>
+      <c r="M26" s="239"/>
+      <c r="N26" s="240"/>
     </row>
     <row r="27" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="33"/>
-      <c r="C27" s="238" t="s">
+      <c r="C27" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
+      <c r="D27" s="241"/>
+      <c r="E27" s="241"/>
       <c r="F27" s="72"/>
       <c r="G27" s="72"/>
       <c r="H27" s="32"/>
-      <c r="I27" s="215"/>
-      <c r="J27" s="217"/>
-      <c r="K27" s="217"/>
-      <c r="L27" s="217"/>
-      <c r="M27" s="217"/>
-      <c r="N27" s="218"/>
+      <c r="I27" s="218"/>
+      <c r="J27" s="220"/>
+      <c r="K27" s="220"/>
+      <c r="L27" s="220"/>
+      <c r="M27" s="220"/>
+      <c r="N27" s="221"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
@@ -12440,7 +12469,7 @@
       <c r="G30" s="72"/>
       <c r="H30" s="32"/>
       <c r="I30" s="33"/>
-      <c r="J30" s="129" t="s">
+      <c r="J30" s="136" t="s">
         <v>49</v>
       </c>
       <c r="K30" s="108"/>
@@ -12473,10 +12502,10 @@
       <c r="H32" s="32"/>
       <c r="I32" s="33"/>
       <c r="J32" s="100"/>
-      <c r="K32" s="239" t="s">
+      <c r="K32" s="261" t="s">
         <v>60</v>
       </c>
-      <c r="L32" s="240"/>
+      <c r="L32" s="262"/>
       <c r="M32" s="105"/>
       <c r="N32" s="32"/>
     </row>
@@ -12505,10 +12534,10 @@
       <c r="H34" s="32"/>
       <c r="I34" s="33"/>
       <c r="J34" s="100"/>
-      <c r="K34" s="249" t="s">
+      <c r="K34" s="263" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="250"/>
+      <c r="L34" s="264"/>
       <c r="M34" s="105"/>
       <c r="N34" s="32"/>
     </row>
@@ -12543,7 +12572,7 @@
       <c r="H36" s="32"/>
       <c r="I36" s="33"/>
       <c r="J36" s="100"/>
-      <c r="K36" s="201" t="s">
+      <c r="K36" s="204" t="s">
         <v>62</v>
       </c>
       <c r="L36" s="10"/>
@@ -12559,12 +12588,12 @@
       <c r="G37" s="10"/>
       <c r="H37" s="32"/>
       <c r="I37" s="33"/>
-      <c r="J37" s="186"/>
-      <c r="K37" s="119" t="s">
+      <c r="J37" s="189"/>
+      <c r="K37" s="120" t="s">
         <v>2</v>
       </c>
       <c r="L37" s="72"/>
-      <c r="M37" s="187"/>
+      <c r="M37" s="190"/>
       <c r="N37" s="32"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -12576,10 +12605,10 @@
       <c r="G38" s="10"/>
       <c r="H38" s="32"/>
       <c r="I38" s="33"/>
-      <c r="J38" s="188"/>
-      <c r="K38" s="189"/>
-      <c r="L38" s="190"/>
-      <c r="M38" s="191"/>
+      <c r="J38" s="191"/>
+      <c r="K38" s="192"/>
+      <c r="L38" s="193"/>
+      <c r="M38" s="194"/>
       <c r="N38" s="32"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
@@ -12613,34 +12642,31 @@
       <c r="N40" s="32"/>
     </row>
     <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="241"/>
-      <c r="C41" s="242"/>
-      <c r="D41" s="243"/>
-      <c r="E41" s="244" t="s">
+      <c r="B41" s="242"/>
+      <c r="C41" s="243"/>
+      <c r="D41" s="244"/>
+      <c r="E41" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="244"/>
-      <c r="G41" s="244"/>
-      <c r="H41" s="245"/>
-      <c r="I41" s="241"/>
-      <c r="J41" s="243"/>
-      <c r="K41" s="244" t="s">
+      <c r="F41" s="245"/>
+      <c r="G41" s="245"/>
+      <c r="H41" s="246"/>
+      <c r="I41" s="242"/>
+      <c r="J41" s="244"/>
+      <c r="K41" s="245" t="s">
         <v>19</v>
       </c>
-      <c r="L41" s="244"/>
-      <c r="M41" s="244"/>
-      <c r="N41" s="245"/>
+      <c r="L41" s="245"/>
+      <c r="M41" s="245"/>
+      <c r="N41" s="246"/>
     </row>
     <row r="42" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="8">
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="K34:L34"/>
@@ -12655,10 +12681,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B1:N42"/>
+  <dimension ref="B1:O42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12667,69 +12693,74 @@
     <col min="3" max="3" width="15.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7" style="7" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="5"/>
     <col min="10" max="10" width="13.140625" style="5" customWidth="1"/>
     <col min="11" max="11" width="18" style="5" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="5"/>
+    <col min="13" max="13" width="6.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="5" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="29" t="s">
         <v>51</v>
       </c>
       <c r="I2" s="41"/>
       <c r="J2" s="41"/>
-      <c r="K2" s="258" t="s">
+      <c r="K2" s="257" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="259" t="s">
+      <c r="L2" s="258" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="188"/>
+    </row>
+    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I3" s="41"/>
       <c r="J3" s="41"/>
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
-    </row>
-    <row r="4" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
       <c r="I4" s="43"/>
       <c r="J4" s="44"/>
       <c r="K4" s="44"/>
       <c r="L4" s="44"/>
-      <c r="M4" s="45"/>
-    </row>
-    <row r="5" spans="2:14" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
+    </row>
+    <row r="5" spans="2:15" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="19"/>
-      <c r="C5" s="160" t="s">
+      <c r="C5" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
       <c r="F5" s="99"/>
       <c r="G5" s="99"/>
       <c r="H5" s="20"/>
       <c r="I5" s="46"/>
-      <c r="J5" s="174" t="s">
+      <c r="J5" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="174"/>
-      <c r="L5" s="174"/>
-      <c r="M5" s="47"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="47"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="21"/>
       <c r="C6" s="13" t="s">
         <v>54</v>
@@ -12757,9 +12788,10 @@
       <c r="L6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="50"/>
-    </row>
-    <row r="7" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="M6" s="98"/>
+      <c r="N6" s="50"/>
+    </row>
+    <row r="7" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B7" s="33"/>
       <c r="C7" s="84">
         <v>0</v>
@@ -12768,25 +12800,26 @@
         <v>5</v>
       </c>
       <c r="E7" s="85"/>
-      <c r="F7" s="85">
+      <c r="F7" s="84">
         <v>0</v>
       </c>
-      <c r="G7" s="201">
+      <c r="G7" s="204">
         <v>1</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="51"/>
-      <c r="J7" s="229">
+      <c r="J7" s="232">
         <v>0</v>
       </c>
-      <c r="K7" s="254" t="s">
+      <c r="K7" s="253" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="205"/>
-      <c r="M7" s="230"/>
-      <c r="N7" s="212"/>
-    </row>
-    <row r="8" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="L7" s="208"/>
+      <c r="M7" s="188"/>
+      <c r="N7" s="233"/>
+      <c r="O7" s="215"/>
+    </row>
+    <row r="8" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B8" s="33"/>
       <c r="C8" s="37">
         <v>1</v>
@@ -12795,7 +12828,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="36"/>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>0</v>
       </c>
       <c r="G8" s="14">
@@ -12803,77 +12836,82 @@
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="51"/>
-      <c r="J8" s="229">
+      <c r="J8" s="232">
         <v>1</v>
       </c>
-      <c r="K8" s="254" t="s">
+      <c r="K8" s="253" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="205"/>
-      <c r="M8" s="230"/>
-      <c r="N8" s="212"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="208"/>
+      <c r="M8" s="188"/>
+      <c r="N8" s="233"/>
+      <c r="O8" s="215"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="33"/>
       <c r="C9" s="86"/>
       <c r="D9" s="91"/>
       <c r="E9" s="91"/>
-      <c r="F9" s="91"/>
-      <c r="G9" s="202"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="205"/>
       <c r="H9" s="30"/>
       <c r="I9" s="51"/>
-      <c r="J9" s="229"/>
-      <c r="K9" s="254"/>
-      <c r="L9" s="205"/>
-      <c r="M9" s="230"/>
-      <c r="N9" s="212"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J9" s="232"/>
+      <c r="K9" s="253"/>
+      <c r="L9" s="208"/>
+      <c r="M9" s="188"/>
+      <c r="N9" s="233"/>
+      <c r="O9" s="215"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="14"/>
       <c r="H10" s="30"/>
       <c r="I10" s="51"/>
-      <c r="J10" s="229"/>
-      <c r="K10" s="254"/>
-      <c r="L10" s="205"/>
-      <c r="M10" s="230"/>
-      <c r="N10" s="212"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J10" s="232"/>
+      <c r="K10" s="253"/>
+      <c r="L10" s="208"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="233"/>
+      <c r="O10" s="215"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="14"/>
       <c r="H11" s="30"/>
       <c r="I11" s="51"/>
-      <c r="J11" s="229"/>
-      <c r="K11" s="254"/>
-      <c r="L11" s="205"/>
-      <c r="M11" s="230"/>
-      <c r="N11" s="212"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J11" s="232"/>
+      <c r="K11" s="253"/>
+      <c r="L11" s="208"/>
+      <c r="M11" s="188"/>
+      <c r="N11" s="233"/>
+      <c r="O11" s="215"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="33"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="14"/>
       <c r="H12" s="30"/>
       <c r="I12" s="51"/>
-      <c r="J12" s="229"/>
-      <c r="K12" s="254"/>
-      <c r="L12" s="205"/>
-      <c r="M12" s="230"/>
-      <c r="N12" s="212"/>
-    </row>
-    <row r="13" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="J12" s="232"/>
+      <c r="K12" s="253"/>
+      <c r="L12" s="208"/>
+      <c r="M12" s="188"/>
+      <c r="N12" s="233"/>
+      <c r="O12" s="215"/>
+    </row>
+    <row r="13" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
       <c r="C13" s="8" t="s">
         <v>1</v>
@@ -12882,7 +12920,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0</v>
       </c>
       <c r="G13" s="14">
@@ -12890,17 +12928,18 @@
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="229" t="s">
+      <c r="J13" s="232" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="254" t="s">
+      <c r="K13" s="253" t="s">
         <v>48</v>
       </c>
-      <c r="L13" s="205"/>
-      <c r="M13" s="230"/>
-      <c r="N13" s="212"/>
-    </row>
-    <row r="14" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="L13" s="208"/>
+      <c r="M13" s="188"/>
+      <c r="N13" s="233"/>
+      <c r="O13" s="215"/>
+    </row>
+    <row r="14" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B14" s="33"/>
       <c r="C14" s="8" t="s">
         <v>2</v>
@@ -12909,7 +12948,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>1</v>
       </c>
       <c r="G14" s="14">
@@ -12920,145 +12959,155 @@
       <c r="J14" s="102"/>
       <c r="K14" s="102"/>
       <c r="L14" s="102"/>
-      <c r="M14" s="230"/>
-      <c r="N14" s="212"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M14" s="102"/>
+      <c r="N14" s="233"/>
+      <c r="O14" s="215"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="33"/>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="14"/>
       <c r="H15" s="32"/>
       <c r="I15" s="65"/>
-      <c r="J15" s="225"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="225"/>
-      <c r="M15" s="230"/>
-      <c r="N15" s="212"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J15" s="228"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="228"/>
+      <c r="M15" s="228"/>
+      <c r="N15" s="233"/>
+      <c r="O15" s="215"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="33"/>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="14"/>
       <c r="H16" s="32"/>
       <c r="I16" s="65"/>
       <c r="J16" s="102"/>
       <c r="K16" s="102"/>
       <c r="L16" s="102"/>
-      <c r="M16" s="230"/>
-      <c r="N16" s="212"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="102"/>
+      <c r="N16" s="233"/>
+      <c r="O16" s="215"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="14"/>
       <c r="H17" s="32"/>
       <c r="I17" s="65"/>
       <c r="J17" s="102"/>
       <c r="K17" s="102"/>
       <c r="L17" s="102"/>
-      <c r="M17" s="230"/>
-      <c r="N17" s="212"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="102"/>
+      <c r="N17" s="233"/>
+      <c r="O17" s="215"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="33"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="14"/>
       <c r="H18" s="32"/>
       <c r="I18" s="65"/>
       <c r="J18" s="102"/>
       <c r="K18" s="102"/>
       <c r="L18" s="102"/>
-      <c r="M18" s="230"/>
-      <c r="N18" s="212"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="102"/>
+      <c r="N18" s="233"/>
+      <c r="O18" s="215"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="33"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="14"/>
       <c r="H19" s="32"/>
       <c r="I19" s="65"/>
       <c r="J19" s="102"/>
       <c r="K19" s="102"/>
       <c r="L19" s="102"/>
-      <c r="M19" s="230"/>
-      <c r="N19" s="212"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M19" s="102"/>
+      <c r="N19" s="233"/>
+      <c r="O19" s="215"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="14"/>
       <c r="H20" s="32"/>
       <c r="I20" s="65"/>
       <c r="J20" s="102"/>
       <c r="K20" s="102"/>
       <c r="L20" s="102"/>
-      <c r="M20" s="230"/>
-      <c r="N20" s="212"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M20" s="102"/>
+      <c r="N20" s="233"/>
+      <c r="O20" s="215"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="33"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="14"/>
       <c r="H21" s="32"/>
       <c r="I21" s="65"/>
-      <c r="J21" s="178"/>
-      <c r="K21" s="178"/>
-      <c r="L21" s="113"/>
-      <c r="M21" s="230"/>
-      <c r="N21" s="212"/>
-    </row>
-    <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="114"/>
+      <c r="M21" s="114"/>
+      <c r="N21" s="233"/>
+      <c r="O21" s="215"/>
+    </row>
+    <row r="22" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="14"/>
       <c r="H22" s="32"/>
       <c r="I22" s="65"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="114"/>
-      <c r="M22" s="230"/>
-      <c r="N22" s="212"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="115"/>
+      <c r="M22" s="115"/>
+      <c r="N22" s="233"/>
+      <c r="O22" s="215"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="14"/>
       <c r="H23" s="32"/>
       <c r="I23" s="65"/>
-      <c r="J23" s="179"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="114"/>
-      <c r="M23" s="230"/>
-      <c r="N23" s="212"/>
-    </row>
-    <row r="24" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="115"/>
+      <c r="M23" s="115"/>
+      <c r="N23" s="233"/>
+      <c r="O23" s="215"/>
+    </row>
+    <row r="24" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
       <c r="C24" s="8" t="s">
         <v>0</v>
@@ -13067,7 +13116,7 @@
         <v>9</v>
       </c>
       <c r="E24" s="9"/>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>1</v>
       </c>
       <c r="G24" s="14">
@@ -13075,62 +13124,66 @@
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="65"/>
-      <c r="J24" s="114"/>
+      <c r="J24" s="115"/>
       <c r="K24" s="94"/>
       <c r="L24" s="94"/>
-      <c r="M24" s="230"/>
-      <c r="N24" s="212"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="94"/>
+      <c r="N24" s="233"/>
+      <c r="O24" s="215"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
       <c r="C25" s="34"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="10"/>
       <c r="H25" s="32"/>
       <c r="I25" s="65"/>
       <c r="J25" s="102"/>
       <c r="K25" s="102"/>
       <c r="L25" s="102"/>
-      <c r="M25" s="230"/>
-      <c r="N25" s="212"/>
-    </row>
-    <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="102"/>
+      <c r="N25" s="233"/>
+      <c r="O25" s="215"/>
+    </row>
+    <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="33"/>
       <c r="C26" s="34"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="10"/>
       <c r="H26" s="32"/>
-      <c r="I26" s="255"/>
-      <c r="J26" s="235"/>
-      <c r="K26" s="256" t="s">
+      <c r="I26" s="254"/>
+      <c r="J26" s="238"/>
+      <c r="K26" s="255" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="256"/>
-      <c r="M26" s="257"/>
-      <c r="N26" s="212"/>
-    </row>
-    <row r="27" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="255"/>
+      <c r="M26" s="255"/>
+      <c r="N26" s="256"/>
+      <c r="O26" s="215"/>
+    </row>
+    <row r="27" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" s="33"/>
-      <c r="C27" s="238" t="s">
+      <c r="C27" s="241" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
+      <c r="D27" s="241"/>
+      <c r="E27" s="241"/>
       <c r="F27" s="72"/>
       <c r="G27" s="72"/>
       <c r="H27" s="32"/>
-      <c r="I27" s="215"/>
-      <c r="J27" s="217"/>
-      <c r="K27" s="217"/>
-      <c r="L27" s="217"/>
-      <c r="M27" s="218"/>
-      <c r="N27" s="212"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I27" s="218"/>
+      <c r="J27" s="220"/>
+      <c r="K27" s="220"/>
+      <c r="L27" s="220"/>
+      <c r="M27" s="220"/>
+      <c r="N27" s="221"/>
+      <c r="O27" s="215"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
       <c r="C28" s="14" t="s">
         <v>46</v>
@@ -13148,10 +13201,11 @@
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="212"/>
-    </row>
-    <row r="29" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="M28" s="10"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="215"/>
+    </row>
+    <row r="29" spans="2:15" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="33"/>
       <c r="C29" s="8">
         <v>0</v>
@@ -13169,10 +13223,11 @@
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="212"/>
-    </row>
-    <row r="30" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="M29" s="10"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="215"/>
+    </row>
+    <row r="30" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="37">
         <v>1</v>
@@ -13187,15 +13242,16 @@
       <c r="G30" s="72"/>
       <c r="H30" s="32"/>
       <c r="I30" s="33"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="181" t="s">
+      <c r="J30" s="133" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="182"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="212"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K30" s="134"/>
+      <c r="L30" s="121"/>
+      <c r="M30" s="122"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="215"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
       <c r="C31" s="8"/>
       <c r="D31" s="9"/>
@@ -13204,13 +13260,14 @@
       <c r="G31" s="34"/>
       <c r="H31" s="32"/>
       <c r="I31" s="33"/>
-      <c r="J31" s="98"/>
-      <c r="K31" s="183"/>
-      <c r="L31" s="184"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="212"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J31" s="123"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="124"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="215"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="33"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
@@ -13219,13 +13276,16 @@
       <c r="G32" s="34"/>
       <c r="H32" s="32"/>
       <c r="I32" s="33"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="212"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J32" s="125"/>
+      <c r="K32" s="259" t="s">
+        <v>60</v>
+      </c>
+      <c r="L32" s="260"/>
+      <c r="M32" s="126"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="215"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="33"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -13234,13 +13294,14 @@
       <c r="G33" s="34"/>
       <c r="H33" s="32"/>
       <c r="I33" s="33"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="212"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J33" s="125"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="126"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="215"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -13249,13 +13310,16 @@
       <c r="G34" s="34"/>
       <c r="H34" s="32"/>
       <c r="I34" s="33"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="212"/>
-    </row>
-    <row r="35" spans="2:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="J34" s="125"/>
+      <c r="K34" s="259" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="260"/>
+      <c r="M34" s="126"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="215"/>
+    </row>
+    <row r="35" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B35" s="33"/>
       <c r="C35" s="8" t="s">
         <v>1</v>
@@ -13270,112 +13334,121 @@
       <c r="G35" s="34"/>
       <c r="H35" s="32"/>
       <c r="I35" s="33"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="212"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J35" s="125"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="126"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="215"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" s="33"/>
       <c r="C36" s="34"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="10"/>
       <c r="H36" s="32"/>
       <c r="I36" s="33"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="212"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J36" s="125"/>
+      <c r="K36" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L36" s="25"/>
+      <c r="M36" s="126"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="215"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="21"/>
       <c r="C37" s="24"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="F37" s="97"/>
       <c r="G37" s="25"/>
       <c r="H37" s="22"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="22"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J37" s="209"/>
+      <c r="K37" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" s="72"/>
+      <c r="M37" s="210"/>
+      <c r="N37" s="22"/>
+    </row>
+    <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21"/>
       <c r="C38" s="71"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="F38" s="97"/>
       <c r="G38" s="25"/>
       <c r="H38" s="22"/>
       <c r="I38" s="21"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="22"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="J38" s="211"/>
+      <c r="K38" s="212"/>
+      <c r="L38" s="213"/>
+      <c r="M38" s="214"/>
+      <c r="N38" s="22"/>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="21"/>
       <c r="C39" s="95"/>
       <c r="D39" s="25"/>
       <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="F39" s="97"/>
       <c r="G39" s="25"/>
       <c r="H39" s="22"/>
       <c r="I39" s="21"/>
       <c r="J39" s="25"/>
       <c r="K39" s="25"/>
       <c r="L39" s="25"/>
-      <c r="M39" s="22"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M39" s="25"/>
+      <c r="N39" s="22"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="21"/>
       <c r="C40" s="24"/>
       <c r="D40" s="25"/>
       <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
+      <c r="F40" s="97"/>
       <c r="G40" s="25"/>
       <c r="H40" s="22"/>
       <c r="I40" s="21"/>
       <c r="J40" s="25"/>
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
-      <c r="M40" s="22"/>
-    </row>
-    <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M40" s="25"/>
+      <c r="N40" s="22"/>
+    </row>
+    <row r="41" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="26"/>
       <c r="C41" s="27"/>
       <c r="D41" s="28"/>
-      <c r="E41" s="162" t="s">
+      <c r="E41" s="169" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="162"/>
-      <c r="G41" s="162"/>
-      <c r="H41" s="163"/>
+      <c r="F41" s="169"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="170"/>
       <c r="I41" s="26"/>
       <c r="J41" s="28"/>
       <c r="K41" s="73" t="s">
         <v>19</v>
       </c>
       <c r="L41" s="73"/>
-      <c r="M41" s="74"/>
-    </row>
-    <row r="42" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="74"/>
+    </row>
+    <row r="42" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="6">
     <mergeCell ref="E41:H41"/>
     <mergeCell ref="J5:L5"/>
-    <mergeCell ref="K30:L31"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C5:E5"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K34:L34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>